<commit_message>
feat: Alteração de arquivos.
</commit_message>
<xml_diff>
--- a/Codigo/preditivo.xlsx
+++ b/Codigo/preditivo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\compiladores\Codigo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A57BEA-C725-41A3-AFC6-7F1D54783039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF1E61F-D0BA-4030-BDCB-415A5C6FFC1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Página1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>S</t>
   </si>
@@ -162,13 +162,16 @@
   </si>
   <si>
     <t>ENQUANTO</t>
+  </si>
+  <si>
+    <t>NT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -201,6 +204,13 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -250,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -262,6 +272,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,8 +493,8 @@
   </sheetPr>
   <dimension ref="A1:AB24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AA10" sqref="AA10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -492,7 +503,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
+      <c r="A1" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="B1" s="5" t="s">
         <v>17</v>
       </c>
@@ -571,7 +584,7 @@
       <c r="AB1" s="4"/>
     </row>
     <row r="2" spans="1:28" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2">

</xml_diff>